<commit_message>
Pbs in TVM hyperplan projection implementation.
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="54">
   <si>
     <t>performance_calculator</t>
   </si>
@@ -153,9 +153,6 @@
     <t>obj.beats_simulation.load_scenario('C:\Users\Felix\code\autoCalibrationProject\beats_scenarios\210E.xml');</t>
   </si>
   <si>
-    <t>[-873337960;128793003]</t>
-  </si>
-  <si>
     <t>knobs.knob_link_ids</t>
   </si>
   <si>
@@ -172,6 +169,15 @@
   </si>
   <si>
     <t>[0]</t>
+  </si>
+  <si>
+    <t>[ -873337960;128793003;-781754904;-128793036;-126537863;-126499580;-24558231;-24029866;-24026218;126499392;756090723]</t>
+  </si>
+  <si>
+    <t>[1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25;1.25]</t>
+  </si>
+  <si>
+    <t>[0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5;0.5]</t>
   </si>
 </sst>
 </file>
@@ -215,10 +221,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,7 +533,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F10" sqref="F10"/>
+      <selection pane="topRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,12 +647,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
         <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -657,19 +666,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -755,7 +764,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>21</v>
@@ -772,7 +781,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>22</v>
@@ -789,13 +798,13 @@
         <v>10</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
@@ -880,7 +889,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
@@ -891,7 +900,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
implementing congestion pattern pc
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
   <si>
     <t>performance_calculator</t>
   </si>
@@ -170,15 +170,6 @@
   </si>
   <si>
     <t>[100]</t>
-  </si>
-  <si>
-    <t>[200]</t>
-  </si>
-  <si>
-    <t>[10]</t>
-  </si>
-  <si>
-    <t>TVM</t>
   </si>
 </sst>
 </file>
@@ -537,7 +528,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +545,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>25</v>
@@ -697,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -825,7 +816,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
stuck with non matching templates and output
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
     <t>performance_calculator</t>
   </si>
@@ -170,6 +170,21 @@
   </si>
   <si>
     <t>[100]</t>
+  </si>
+  <si>
+    <t>knobs.overevaluation_tolerance_coefficient</t>
+  </si>
+  <si>
+    <t>knobs.underevaluation_tolerance_coefficient</t>
+  </si>
+  <si>
+    <t>[1.5]</t>
+  </si>
+  <si>
+    <t>[0.5]</t>
+  </si>
+  <si>
+    <t>isnaive_knob_boundaries</t>
   </si>
 </sst>
 </file>
@@ -238,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -280,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -524,14 +539,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B21" sqref="B21"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.7109375" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" customWidth="1"/>
@@ -624,231 +639,255 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" t="s">
-        <v>27</v>
+        <v>8</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="s">
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
errorfunction is now an object, knobs will be made an object too
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
-  <si>
-    <t>error_calculator</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
     <t>knobs.knob_boundaries_min</t>
   </si>
@@ -55,9 +52,6 @@
     <t>normopts.SIGMAS</t>
   </si>
   <si>
-    <t>L2</t>
-  </si>
-  <si>
     <t>[0.5;0.5]</t>
   </si>
   <si>
@@ -226,13 +220,16 @@
     <t>temp.congestion_patterns{2,1}.down_ordinate</t>
   </si>
   <si>
-    <t>temp.perfStruct</t>
-  </si>
-  <si>
     <t>Utilities.char2char('C:\Users\Felix\code\autoCalibrationProject\config\210E_joined_frmode_beats.xml')</t>
   </si>
   <si>
     <t>struct('CongestionPattern',0.3,'TVM',0.4,'TVH',0.3)</t>
+  </si>
+  <si>
+    <t>temp.erfStruct.performance_calculators</t>
+  </si>
+  <si>
+    <t>temp.erfStruct.error_calculator</t>
   </si>
 </sst>
 </file>
@@ -336,7 +333,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -378,7 +375,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -413,7 +410,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -622,14 +619,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" style="3" customWidth="1"/>
@@ -641,415 +638,407 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>2</v>
+        <v>64</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="B29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="5"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>47</v>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="5"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="B37" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Knobs is now a class
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -16,12 +16,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="72">
   <si>
-    <t>knobs.knob_boundaries_min</t>
-  </si>
-  <si>
-    <t>knobs.knob_boundaries_max</t>
-  </si>
-  <si>
     <t>maxEval</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t>Utilities.char2char('C:\Users\Felix\code\autoCalibrationProject\pems_test\processed')</t>
   </si>
   <si>
-    <t>knobs.knob_link_ids</t>
-  </si>
-  <si>
     <t>[4]</t>
   </si>
   <si>
@@ -139,9 +130,6 @@
     <t>[300]</t>
   </si>
   <si>
-    <t>force_manual_knob_boundaries</t>
-  </si>
-  <si>
     <t>[0]</t>
   </si>
   <si>
@@ -172,9 +160,6 @@
     <t>[0.5]</t>
   </si>
   <si>
-    <t>isnaive_knob_boundaries</t>
-  </si>
-  <si>
     <t>cell(2,1)</t>
   </si>
   <si>
@@ -230,6 +215,21 @@
   </si>
   <si>
     <t>temp.erfStruct.error_calculator</t>
+  </si>
+  <si>
+    <t>knobs.link_ids</t>
+  </si>
+  <si>
+    <t>knobs.force_manual_knob_boundaries</t>
+  </si>
+  <si>
+    <t>knobs.boundaries_min</t>
+  </si>
+  <si>
+    <t>knobs.boundaries_max</t>
+  </si>
+  <si>
+    <t>knobs.isnaive_boundaries</t>
   </si>
 </sst>
 </file>
@@ -621,9 +621,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8:A11"/>
+      <selection pane="topRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,300 +638,300 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -942,98 +942,98 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E38" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
knobs, pems and errorfunction are now AlgorithmBox-dependent objects for better code clarity
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -619,11 +619,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A21" sqref="A21"/>
+      <selection pane="topRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,40 +670,31 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
@@ -711,334 +702,343 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>71</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>69</v>
+        <v>45</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>46</v>
+        <v>19</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="5"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="A35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E41" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="1"/>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working great with beats as pems, interface is done except some probable bugs
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="9540" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="cmaes" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>[1.2,0.8;1.1,0.9]</t>
   </si>
   <si>
-    <t>[2]</t>
-  </si>
-  <si>
     <t>pems.days</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>[1.5]</t>
   </si>
   <si>
-    <t>[0.5]</t>
-  </si>
-  <si>
     <t>temp.congestion_patterns</t>
   </si>
   <si>
@@ -235,13 +229,19 @@
     <t>[220]</t>
   </si>
   <si>
-    <t>struct('CongestionPattern',0.9999,'TVH',0.0001)</t>
-  </si>
-  <si>
     <t>[10]</t>
   </si>
   <si>
-    <t>[6000]</t>
+    <t>struct('CongestionPattern',[0.9989,1],'TVH',[0.001,2],'TVM',[0.0001,2])</t>
+  </si>
+  <si>
+    <t>[100]</t>
+  </si>
+  <si>
+    <t>[0.9]</t>
+  </si>
+  <si>
+    <t>[1.1]</t>
   </si>
 </sst>
 </file>
@@ -633,9 +633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B28" sqref="B28"/>
+      <selection pane="topRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -650,114 +650,114 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -771,60 +771,60 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -883,7 +883,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
@@ -900,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>13</v>
@@ -917,7 +917,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>14</v>
@@ -934,13 +934,13 @@
         <v>5</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>11</v>
@@ -957,7 +957,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>15</v>
@@ -1017,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>11</v>
@@ -1031,7 +1031,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>17</v>
@@ -1042,7 +1042,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
branch working using 210E_joined_frmode_beats.xml
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10470" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="cmaes" sheetId="1" r:id="rId1"/>
@@ -163,9 +163,6 @@
     <t>temp.congestion_patterns{1,1}.down_ordinate</t>
   </si>
   <si>
-    <t>Utilities.char2char('C:\Users\Felix\code\autoCalibrationProject\config\210E_joined_frmode_beats.xml')</t>
-  </si>
-  <si>
     <t>temp.erfStruct.performance_calculators</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>[10]</t>
   </si>
   <si>
-    <t>struct('CongestionPattern',[0.9989,1],'TVH',[0.001,2],'TVM',[0.0001,2])</t>
-  </si>
-  <si>
     <t>[100]</t>
   </si>
   <si>
@@ -242,6 +236,12 @@
   </si>
   <si>
     <t>[1.1]</t>
+  </si>
+  <si>
+    <t>struct('CongestionPattern',[0.34,1],'TVH',[0.33,1],'TVM',[0.33,1])</t>
+  </si>
+  <si>
+    <t>Utilities.char2char('C:\Users\Felix\code\autoCalibrationProject\config\210E_joined_frmode.xml')</t>
   </si>
 </sst>
 </file>
@@ -633,9 +633,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B34" sqref="B34"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,7 @@
         <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,7 +685,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -701,7 +701,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>47</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -717,47 +717,47 @@
         <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -771,15 +771,15 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>37</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>36</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>36</v>
@@ -803,12 +803,12 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>42</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>41</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -849,7 +849,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>11</v>
@@ -866,7 +866,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>11</v>
@@ -1017,7 +1017,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
small improvements in movies
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="30930" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="cmaes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="71">
   <si>
     <t>maxEval</t>
   </si>
@@ -205,15 +205,9 @@
     <t>[2]</t>
   </si>
   <si>
-    <t>[2.5]</t>
-  </si>
-  <si>
     <t>[3]</t>
   </si>
   <si>
-    <t>[3.5]</t>
-  </si>
-  <si>
     <t>Utilities.char2char('C:\Users\Felix\code\autoCalibrationProject\config\210E_joined.xml')</t>
   </si>
   <si>
@@ -230,6 +224,9 @@
   </si>
   <si>
     <t>[1000]</t>
+  </si>
+  <si>
+    <t>[5]</t>
   </si>
 </sst>
 </file>
@@ -332,7 +329,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -374,7 +371,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,7 +406,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -618,86 +615,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U60"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" style="2" customWidth="1"/>
-    <col min="3" max="6" width="31.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="75.7109375" style="2" customWidth="1"/>
-    <col min="8" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="75.7109375" style="2" customWidth="1"/>
-    <col min="12" max="15" width="31.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="75.7109375" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="5" width="31.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="2" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="35.7109375" style="2" customWidth="1"/>
+    <col min="11" max="13" width="31.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -749,14 +740,8 @@
       <c r="Q2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
@@ -808,14 +793,8 @@
       <c r="Q3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
@@ -867,14 +846,8 @@
       <c r="Q4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -926,14 +899,8 @@
       <c r="Q5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
@@ -985,14 +952,8 @@
       <c r="Q6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>34</v>
       </c>
@@ -1044,14 +1005,8 @@
       <c r="Q7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="R7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>35</v>
       </c>
@@ -1103,14 +1058,8 @@
       <c r="Q8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -1162,14 +1111,8 @@
       <c r="Q9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>50</v>
       </c>
@@ -1221,14 +1164,8 @@
       <c r="Q10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="R10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>51</v>
       </c>
@@ -1280,14 +1217,8 @@
       <c r="Q11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S11" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>52</v>
       </c>
@@ -1339,14 +1270,8 @@
       <c r="Q12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="R12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="S12" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -1398,73 +1323,61 @@
       <c r="Q13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
@@ -1516,30 +1429,22 @@
       <c r="Q15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-    </row>
-    <row r="17" spans="1:21" ht="300" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" ht="300" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1591,14 +1496,8 @@
       <c r="Q17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1650,14 +1549,8 @@
       <c r="Q18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>43</v>
       </c>
@@ -1709,52 +1602,42 @@
       <c r="Q19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
       <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
       <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>31</v>
       </c>
@@ -1783,37 +1666,31 @@
         <v>60</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>30</v>
       </c>
@@ -1842,53 +1719,45 @@
         <v>59</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
       <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
-      <c r="R24" s="2"/>
-      <c r="S24" s="2"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -1940,75 +1809,62 @@
       <c r="Q25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="R25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T26" s="2"/>
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="R26" s="2"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>1</v>
       </c>
@@ -2060,14 +1916,8 @@
       <c r="Q27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="R27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
@@ -2119,30 +1969,22 @@
       <c r="Q28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S28" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
       <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
-      <c r="S29" s="2"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2194,14 +2036,8 @@
       <c r="Q30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R30" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="S30" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
@@ -2253,14 +2089,8 @@
       <c r="Q31" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R31" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="S31" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
@@ -2312,14 +2142,8 @@
       <c r="Q32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="R32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="S32" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2336,10 +2160,8 @@
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
@@ -2350,55 +2172,49 @@
         <v>63</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="I34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K34" s="2" t="s">
+      <c r="L34" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="O34" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="O34" s="2" t="s">
+      <c r="P34" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P34" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="Q34" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S34" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
@@ -2450,14 +2266,8 @@
       <c r="Q35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S35" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>15</v>
       </c>
@@ -2509,14 +2319,8 @@
       <c r="Q36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="R36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>7</v>
       </c>
@@ -2568,14 +2372,8 @@
       <c r="Q37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R37" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>8</v>
       </c>
@@ -2627,14 +2425,8 @@
       <c r="Q38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R38" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>9</v>
       </c>
@@ -2686,19 +2478,13 @@
       <c r="Q39" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="S39" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="P60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="N60" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on using pems data
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="32790" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="cmaes" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="72">
   <si>
     <t>maxEval</t>
   </si>
@@ -37,9 +37,6 @@
     <t>insigma</t>
   </si>
   <si>
-    <t>population_size</t>
-  </si>
-  <si>
     <t>normopts.CENTERS</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>[220]</t>
   </si>
   <si>
-    <t>[10]</t>
-  </si>
-  <si>
     <t>[1.3]</t>
   </si>
   <si>
@@ -227,6 +221,15 @@
   </si>
   <si>
     <t>[100]</t>
+  </si>
+  <si>
+    <t>[ -873337960;-781754904;-126537863;-126499580;-24558231;-24029866;-24026218;126499392]</t>
+  </si>
+  <si>
+    <t>[8]</t>
+  </si>
+  <si>
+    <t>initial_population_size</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -371,7 +374,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -406,7 +409,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -615,20 +618,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P37" sqref="P37:S37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" style="2" customWidth="1"/>
     <col min="3" max="5" width="31.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" style="2" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="7" max="7" width="23.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="35.7109375" style="2" customWidth="1"/>
     <col min="11" max="13" width="31.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="29.28515625" style="2" customWidth="1"/>
@@ -637,797 +641,797 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1444,168 +1448,183 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:18" ht="300" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="240" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="U17" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1620,9 +1639,9 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1637,113 +1656,113 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1757,220 +1776,220 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1984,166 +2003,166 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
@@ -2161,322 +2180,328 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="B36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q37" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="B38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K38" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="M39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O38" s="2" t="s">
+      <c r="O39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="P38" s="2" t="s">
+      <c r="P39" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="Q39" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q39" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Knobs tuning ready. Still to do: fix plots mostly
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -262,9 +262,6 @@
     <t>[0.025]</t>
   </si>
   <si>
-    <t>struct('CongestionPattern',[0.33],'TVH',[0.33],'KnobsDistance',[0.34],'TVM',[0])</t>
-  </si>
-  <si>
     <t>['uniform']</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>error_function.pcs_uncertainty</t>
+  </si>
+  <si>
+    <t>struct('CongestionPattern',[0.5],'TVH',[0.25],'KnobsDistance',[0.25],'TVM',[0])</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
   <dimension ref="A1:Y71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +775,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>40</v>
@@ -1006,7 +1006,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>41</v>
@@ -1234,7 +1234,7 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B7" s="10"/>
     </row>
@@ -1830,76 +1830,76 @@
         <v>63</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="P23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="R23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="S23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="T23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="U23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="V23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="X23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y23" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="P23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="R23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="U23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="V23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="W23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="X23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y23" s="12" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="3"/>
@@ -3103,76 +3103,76 @@
         <v>12</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="V42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Y42" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bugfix. Pcs_uncertainty in excel cannot be set for now
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -757,15 +757,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="116.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="62.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="2" customWidth="1"/>
     <col min="3" max="25" width="75.7109375" style="2" customWidth="1"/>
     <col min="26" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1825,7 +1825,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>63</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
commit before I leave
</commit_message>
<xml_diff>
--- a/xls/Cmaes_210E_program.xlsx
+++ b/xls/Cmaes_210E_program.xlsx
@@ -771,7 +771,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B20" sqref="B20"/>
+      <selection pane="topRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,7 +1110,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>80</v>
@@ -2417,7 +2417,7 @@
         <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>33</v>
@@ -2497,7 +2497,7 @@
         <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>77</v>

</xml_diff>